<commit_message>
Updated Folders and Results
</commit_message>
<xml_diff>
--- a/Results/Bandit.xlsx
+++ b/Results/Bandit.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Frequency" sheetId="1" r:id="rId1"/>
+    <sheet name="Detailed Result" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Model</t>
   </si>
@@ -51,6 +52,78 @@
   </si>
   <si>
     <t>GPT 3.5 Turbo with Instruction Tone Prompt</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Issue Severity</t>
+  </si>
+  <si>
+    <t>Issue CWE</t>
+  </si>
+  <si>
+    <t>sample_data/Human_Eval_Dataset/Dataset/105.py</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>sample_data/Human_Eval_Dataset/Dataset/160.py</t>
+  </si>
+  <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>sample_data/Human_Eval_Dataset/Dataset/162.py</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>GPT 3.5 S</t>
+  </si>
+  <si>
+    <t>sample_data/GPT_3.5_Simple_Prompts/Dataset/162.py</t>
+  </si>
+  <si>
+    <t>GPT 3.5 I</t>
+  </si>
+  <si>
+    <t>sample_data/GPT_3.5_Instruction_Tone_Prompt/Dataset/162.py</t>
+  </si>
+  <si>
+    <t>GPT 3.5 E</t>
+  </si>
+  <si>
+    <t>sample_data/GPT_3.5_Turbo_Enhanced_Prompt/Dataset/160.py</t>
+  </si>
+  <si>
+    <t>sample_data/GPT_3.5_Turbo_Enhanced_Prompt/Dataset/162.py</t>
+  </si>
+  <si>
+    <t>GPT 4 S</t>
+  </si>
+  <si>
+    <t>sample_data/GPT_4_Simple_Prompt/Dataset/162.py</t>
+  </si>
+  <si>
+    <t>GPT 4 I</t>
+  </si>
+  <si>
+    <t>sample_data/GPT_4_Instruction_Tone_Prompt/Dataset/160.py</t>
+  </si>
+  <si>
+    <t>sample_data/GPT_4_Instruction_Tone_Prompt/Dataset/162.py</t>
+  </si>
+  <si>
+    <t>GPT 4 E</t>
+  </si>
+  <si>
+    <t>sample_data/GPT_4_Enhanced_Prompt/Dataset/162.py</t>
   </si>
 </sst>
 </file>
@@ -82,7 +155,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -105,11 +178,307 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -117,6 +486,75 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,4 +915,190 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="57.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="10">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="13">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="14"/>
+      <c r="B4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="16">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="7">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="7">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="10">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="16">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="20">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="10">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="21"/>
+      <c r="B11" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="23">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="27">
+        <v>327</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A10:A11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>